<commit_message>
Update reinforcement line format to 4-point tension distribution system
  - Replace FL/FT with T parameter in new Excel 20-row table format
  - Implement 4-point lines with pullout lengths (Lp1/Lp2) and max tension (Tmax)
  - Add E and nu parameters to materials for stress analysis
  - Update slice.py and solve.py to use T instead of FL for reinforcement
  - Add validation with clear error messages for missing parameters
</commit_message>
<xml_diff>
--- a/inputs/slope/input_template_MASTER5.xlsx
+++ b/inputs/slope/input_template_MASTER5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jones/CursorProjects/xslope/inputs/slope/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A422B8-4289-464A-9C5B-C89127F6740D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FF17C7-996E-AC4A-AC6F-72C3AC16E9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="29340" windowHeight="17300" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="29340" windowHeight="17300" activeTab="8" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -5623,7 +5623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02E090B-D957-7046-AD33-44E170F709C1}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -6572,16 +6572,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="M4:N4"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="J22:K22"/>
     <mergeCell ref="M22:N22"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="M4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8330,8 +8330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C4F752-BCE4-AE4E-BC09-D828329F219B}">
   <dimension ref="A2:J25"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8388,9 +8388,15 @@
       <c r="E3" s="3">
         <v>240</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="F3" s="3">
+        <v>2000</v>
+      </c>
+      <c r="G3" s="3">
+        <v>10</v>
+      </c>
+      <c r="H3" s="3">
+        <v>10</v>
+      </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
@@ -8410,9 +8416,15 @@
       <c r="E4" s="3">
         <v>255</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="F4" s="3">
+        <v>2000</v>
+      </c>
+      <c r="G4" s="3">
+        <v>10</v>
+      </c>
+      <c r="H4" s="3">
+        <v>10</v>
+      </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
@@ -8432,9 +8444,15 @@
       <c r="E5" s="3">
         <v>270</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="F5" s="3">
+        <v>2000</v>
+      </c>
+      <c r="G5" s="3">
+        <v>10</v>
+      </c>
+      <c r="H5" s="3">
+        <v>10</v>
+      </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
@@ -8454,9 +8472,15 @@
       <c r="E6" s="3">
         <v>285</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="F6" s="3">
+        <v>2000</v>
+      </c>
+      <c r="G6" s="3">
+        <v>10</v>
+      </c>
+      <c r="H6" s="3">
+        <v>10</v>
+      </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
@@ -8476,9 +8500,15 @@
       <c r="E7" s="3">
         <v>300</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="F7" s="3">
+        <v>2000</v>
+      </c>
+      <c r="G7" s="3">
+        <v>10</v>
+      </c>
+      <c r="H7" s="3">
+        <v>10</v>
+      </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>

</xml_diff>